<commit_message>
Buttons & Entries are partially implemented
</commit_message>
<xml_diff>
--- a/TestSheet.xlsx
+++ b/TestSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbui\Desktop\TrendingProg\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbui\Desktop\TrendingProg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17130" windowHeight="7860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9765" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>